<commit_message>
Controladores fachada e conexao
</commit_message>
<xml_diff>
--- a/01_Diretrizes_Projeto_Implementacao_MyGym.xlsx
+++ b/01_Diretrizes_Projeto_Implementacao_MyGym.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
   <si>
     <t>Artefatos / Documentos</t>
   </si>
@@ -561,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -692,6 +692,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,7 +1000,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1219,6 +1220,9 @@
       <c r="C19" s="41" t="s">
         <v>42</v>
       </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
@@ -1239,6 +1243,7 @@
       <c r="C21" s="45" t="s">
         <v>28</v>
       </c>
+      <c r="D21" s="46"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8">

</xml_diff>

<commit_message>
Formulario I - Aluno
</commit_message>
<xml_diff>
--- a/01_Diretrizes_Projeto_Implementacao_MyGym.xlsx
+++ b/01_Diretrizes_Projeto_Implementacao_MyGym.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>Artefatos / Documentos</t>
   </si>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1308,6 +1308,9 @@
         <v>45</v>
       </c>
       <c r="C28" s="19"/>
+      <c r="D28" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
@@ -1324,6 +1327,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="18"/>
+      <c r="D30" s="46"/>
     </row>
     <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>

</xml_diff>

<commit_message>
povoamento simplificado para BIRT
</commit_message>
<xml_diff>
--- a/01_Diretrizes_Projeto_Implementacao_MyGym.xlsx
+++ b/01_Diretrizes_Projeto_Implementacao_MyGym.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>Artefatos / Documentos</t>
   </si>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1392,6 +1392,9 @@
       <c r="C37" s="34" t="s">
         <v>38</v>
       </c>
+      <c r="D37" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>

</xml_diff>